<commit_message>
made comment on key point covered
</commit_message>
<xml_diff>
--- a/ArrayLiteralsAndMonthFirstLastDays.xlsx
+++ b/ArrayLiteralsAndMonthFirstLastDays.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16BDBE3D-1A02-4095-B44E-BDC023DE6F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6284F4DB-E6DF-4B33-AA53-6916F025860D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31515" yWindow="1290" windowWidth="21600" windowHeight="12675" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>FROM:</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>All in One</t>
+  </si>
+  <si>
+    <t>Notice how the sequence broadcasts across the array.</t>
   </si>
 </sst>
 </file>
@@ -96,7 +99,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]d/mmm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yy;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -258,7 +261,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -581,7 +584,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -628,6 +631,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
@@ -757,13 +765,11 @@
         <f t="array" ref="C15:C26">EOMONTH(C9,_xlfn.SEQUENCE(12,,0))</f>
         <v>44408</v>
       </c>
-      <c r="E15" s="4" cm="1">
-        <f t="array" ref="E15:F26">EOMONTH(C9,{-1,0}+_xlfn.SEQUENCE(12,,0))+{1,0}</f>
-        <v>44378</v>
-      </c>
-      <c r="F15" s="4">
-        <v>44408</v>
-      </c>
+      <c r="E15" s="4">
+        <f>E8</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="4"/>
       <c r="I15">
         <v>4</v>
       </c>
@@ -788,12 +794,8 @@
       <c r="C16" s="4">
         <v>44439</v>
       </c>
-      <c r="E16" s="4">
-        <v>44409</v>
-      </c>
-      <c r="F16" s="4">
-        <v>44439</v>
-      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="I16">
         <v>5</v>
       </c>
@@ -818,12 +820,8 @@
       <c r="C17" s="4">
         <v>44469</v>
       </c>
-      <c r="E17" s="4">
-        <v>44440</v>
-      </c>
-      <c r="F17" s="4">
-        <v>44469</v>
-      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="I17">
         <v>6</v>
       </c>
@@ -848,12 +846,8 @@
       <c r="C18" s="4">
         <v>44500</v>
       </c>
-      <c r="E18" s="4">
-        <v>44470</v>
-      </c>
-      <c r="F18" s="4">
-        <v>44500</v>
-      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
       <c r="I18">
         <v>7</v>
       </c>
@@ -878,12 +872,8 @@
       <c r="C19" s="4">
         <v>44530</v>
       </c>
-      <c r="E19" s="4">
-        <v>44501</v>
-      </c>
-      <c r="F19" s="4">
-        <v>44530</v>
-      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
       <c r="I19">
         <v>8</v>
       </c>
@@ -908,12 +898,8 @@
       <c r="C20" s="4">
         <v>44561</v>
       </c>
-      <c r="E20" s="4">
-        <v>44531</v>
-      </c>
-      <c r="F20" s="4">
-        <v>44561</v>
-      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
       <c r="I20">
         <v>9</v>
       </c>
@@ -938,12 +924,8 @@
       <c r="C21" s="4">
         <v>44592</v>
       </c>
-      <c r="E21" s="4">
-        <v>44562</v>
-      </c>
-      <c r="F21" s="4">
-        <v>44592</v>
-      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
       <c r="I21">
         <v>10</v>
       </c>
@@ -968,12 +950,8 @@
       <c r="C22" s="4">
         <v>44620</v>
       </c>
-      <c r="E22" s="4">
-        <v>44593</v>
-      </c>
-      <c r="F22" s="4">
-        <v>44620</v>
-      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
@@ -982,12 +960,8 @@
       <c r="C23" s="4">
         <v>44651</v>
       </c>
-      <c r="E23" s="4">
-        <v>44621</v>
-      </c>
-      <c r="F23" s="4">
-        <v>44651</v>
-      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
@@ -996,12 +970,8 @@
       <c r="C24" s="4">
         <v>44681</v>
       </c>
-      <c r="E24" s="4">
-        <v>44652</v>
-      </c>
-      <c r="F24" s="4">
-        <v>44681</v>
-      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
@@ -1010,12 +980,8 @@
       <c r="C25" s="4">
         <v>44712</v>
       </c>
-      <c r="E25" s="4">
-        <v>44682</v>
-      </c>
-      <c r="F25" s="4">
-        <v>44712</v>
-      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
@@ -1024,12 +990,8 @@
       <c r="C26" s="4">
         <v>44742</v>
       </c>
-      <c r="E26" s="4">
-        <v>44713</v>
-      </c>
-      <c r="F26" s="4">
-        <v>44742</v>
-      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>